<commit_message>
added decay factor in transmission
</commit_message>
<xml_diff>
--- a/data-input/estimated_variables.xlsx
+++ b/data-input/estimated_variables.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
   <si>
     <t>Module</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t>Number of workers clearing</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Survival of bacteria over the 60-minutes</t>
+  </si>
+  <si>
+    <t>proportion</t>
   </si>
 </sst>
 </file>
@@ -656,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P63"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -667,12 +676,13 @@
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" customWidth="1"/>
     <col min="3" max="3" width="18.6328125" customWidth="1"/>
-    <col min="4" max="4" width="56.90625" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7265625" customWidth="1"/>
     <col min="7" max="7" width="10.36328125" customWidth="1"/>
     <col min="8" max="9" width="9.54296875" customWidth="1"/>
-    <col min="10" max="11" width="8.54296875" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.54296875" customWidth="1"/>
     <col min="15" max="15" width="34.1796875" customWidth="1"/>
     <col min="16" max="16" width="54" customWidth="1"/>
   </cols>
@@ -891,44 +901,45 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>47</v>
+    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H6" s="2">
-        <v>7</v>
+        <v>1E-3</v>
       </c>
       <c r="I6" s="2">
-        <v>9</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="J6" s="3">
+        <v>8.6E-3</v>
+      </c>
+      <c r="K6" s="2">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" t="s">
-        <v>50</v>
-      </c>
-      <c r="P6" s="18" t="s">
-        <v>56</v>
-      </c>
+      <c r="O6"/>
+      <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
@@ -938,38 +949,38 @@
         <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="3">
-        <v>3</v>
-      </c>
-      <c r="I7" s="3">
-        <v>13</v>
-      </c>
-      <c r="J7" s="3">
-        <v>6</v>
-      </c>
+      <c r="H7" s="2">
+        <v>7</v>
+      </c>
+      <c r="I7" s="2">
+        <v>9</v>
+      </c>
+      <c r="J7" s="3"/>
       <c r="K7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" t="s">
-        <v>52</v>
-      </c>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>57</v>
       </c>
@@ -977,47 +988,73 @@
         <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H8" s="3">
+        <v>3</v>
+      </c>
+      <c r="I8" s="3">
+        <v>13</v>
+      </c>
+      <c r="J8" s="3">
+        <v>6</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="3">
         <v>20</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I9" s="3">
         <v>30</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="L8"/>
-      <c r="O8" t="s">
+      <c r="J9" s="3"/>
+      <c r="L9"/>
+      <c r="O9" t="s">
         <v>54</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="8"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
@@ -1034,33 +1071,28 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="9"/>
+      <c r="B11" s="8"/>
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="3"/>
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="9"/>
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1080,7 +1112,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="3"/>
@@ -1098,7 +1130,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="L14" s="3"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="3"/>
@@ -1111,10 +1143,10 @@
       <c r="D15" s="10"/>
       <c r="E15" s="9"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1128,16 +1160,17 @@
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
+      <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
@@ -1145,16 +1178,16 @@
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
@@ -1163,7 +1196,7 @@
       <c r="D18" s="10"/>
       <c r="E18" s="9"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="3"/>
@@ -1172,7 +1205,6 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
@@ -1182,15 +1214,15 @@
       <c r="E19" s="9"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
       <c r="J19" s="3"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="5"/>
+      <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
@@ -1218,15 +1250,15 @@
       <c r="E21" s="9"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="2"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
@@ -1272,9 +1304,9 @@
       <c r="E24" s="9"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
@@ -1300,13 +1332,23 @@
       <c r="O25" s="8"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="13"/>
-      <c r="O26" s="3"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
@@ -1314,55 +1356,45 @@
       <c r="C27" s="13"/>
       <c r="D27" s="14"/>
       <c r="E27" s="13"/>
-      <c r="G27" s="3"/>
-      <c r="J27" s="3"/>
       <c r="O27" s="3"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="2"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="13"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="J28" s="3"/>
       <c r="O28" s="3"/>
-      <c r="P28" s="2"/>
-    </row>
-    <row r="29" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="13"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="2"/>
       <c r="G29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
       <c r="O29" s="3"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="13"/>
+      <c r="G30" s="3"/>
+      <c r="J30" s="3"/>
       <c r="O30" s="3"/>
-      <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
@@ -1388,7 +1420,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="3"/>
+      <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -1406,10 +1438,11 @@
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
       <c r="E33" s="9"/>
-      <c r="F33" s="2"/>
+      <c r="F33" s="3"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
@@ -1427,7 +1460,6 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
@@ -1435,30 +1467,31 @@
       <c r="O34" s="3"/>
       <c r="P34" s="2"/>
     </row>
-    <row r="35" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="13"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
       <c r="O35" s="3"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="13"/>
       <c r="O36" s="3"/>
-      <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
@@ -1467,7 +1500,7 @@
       <c r="D37" s="10"/>
       <c r="E37" s="9"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="3"/>
+      <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="K37" s="2"/>
@@ -1488,7 +1521,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="L38" s="3"/>
+      <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="3"/>
@@ -1521,9 +1554,8 @@
       <c r="G40" s="3"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
+      <c r="L40" s="3"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="3"/>
@@ -1562,6 +1594,7 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
+      <c r="O42" s="3"/>
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.35">
@@ -1606,11 +1639,11 @@
       <c r="E45" s="9"/>
       <c r="F45" s="2"/>
       <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-      <c r="L45" s="3"/>
+      <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="P45" s="2"/>
@@ -1618,19 +1651,18 @@
     <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="13"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="9"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="3"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
-      <c r="O46" s="3"/>
       <c r="P46" s="2"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.35">
@@ -1638,9 +1670,9 @@
       <c r="B47" s="3"/>
       <c r="C47" s="13"/>
       <c r="D47" s="14"/>
-      <c r="E47" s="9"/>
+      <c r="E47" s="13"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -1648,34 +1680,35 @@
       <c r="L47" s="3"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
+      <c r="O47" s="3"/>
       <c r="P47" s="2"/>
     </row>
-    <row r="48" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="13"/>
       <c r="D48" s="14"/>
-      <c r="E48" s="13"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="2"/>
       <c r="G48" s="3"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
       <c r="L48" s="3"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+    </row>
+    <row r="49" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="2"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="13"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="P49" s="2"/>
+      <c r="L49" s="3"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
@@ -1689,7 +1722,7 @@
       <c r="I50" s="2"/>
       <c r="J50" s="3"/>
       <c r="K50" s="2"/>
-      <c r="L50" s="3"/>
+      <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="P50" s="2"/>
@@ -1721,9 +1754,9 @@
       <c r="G52" s="3"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
+      <c r="J52" s="3"/>
       <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
+      <c r="L52" s="3"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="P52" s="2"/>
@@ -1738,7 +1771,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
-      <c r="J53" s="3"/>
+      <c r="J53" s="2"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
@@ -1797,12 +1830,26 @@
       <c r="P56" s="2"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
+      <c r="P57" s="2"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="K59" s="2"/>
@@ -1812,52 +1859,55 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="K61" s="2"/>
-      <c r="O61" s="2"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="K62" s="2"/>
       <c r="O62" s="2"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K63" s="2"/>
       <c r="O63" s="2"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O64" s="2"/>
     </row>
   </sheetData>
   <dataValidations xWindow="721" yWindow="594" count="12">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K58:K62">
-      <formula1>I58</formula1>
-      <formula2>J58</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K59:K63">
+      <formula1>I59</formula1>
+      <formula2>J59</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O62">
-      <formula1>K62</formula1>
-      <formula2>L62</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O63">
+      <formula1>K63</formula1>
+      <formula2>L63</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K17:K56 K2:K15">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K18:K57 K2:K16">
       <formula1>I2</formula1>
       <formula2>J2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="P16">
-      <formula1>O16</formula1>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="P17">
+      <formula1>O17</formula1>
       <formula2>#REF!</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L34:L35 L40:L56 L2:L32"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="L37">
-      <formula1>H37</formula1>
-      <formula2>I37</formula2>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L35:L36 L41:L57 L2:L33"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="L38">
+      <formula1>H38</formula1>
+      <formula2>I38</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J34:J35 J40:J56 J2:J32">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J35:J36 J41:J57 J2:J33">
       <formula1>H2</formula1>
       <formula2>I2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="L38:L39 L36 L33">
-      <formula1>H33</formula1>
-      <formula2>I33</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="L39:L40 L37 L34">
+      <formula1>H34</formula1>
+      <formula2>I34</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M56"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N56"/>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I56">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M57"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N57"/>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I57">
       <formula1>H2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H56">
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H57">
       <formula1>I2</formula1>
     </dataValidation>
   </dataValidations>
@@ -1870,13 +1920,13 @@
           <x14:formula1>
             <xm:f>ListItem!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G56</xm:sqref>
+          <xm:sqref>G2:G57</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution" prompt="Select a probability distribution">
           <x14:formula1>
             <xm:f>ListItem!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F56</xm:sqref>
+          <xm:sqref>F2:F57</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
updated with abattoire visit info
</commit_message>
<xml_diff>
--- a/data-input/estimated_variables.xlsx
+++ b/data-input/estimated_variables.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="79">
   <si>
     <t>Module</t>
   </si>
@@ -195,30 +195,12 @@
     <t>Huneau Salaun et al. (2019)</t>
   </si>
   <si>
-    <t>n_slaughter</t>
-  </si>
-  <si>
-    <t>Expert opinion Alfredo</t>
-  </si>
-  <si>
-    <t>To verify</t>
-  </si>
-  <si>
     <t>24000 broilers are treated by 7-9 workers</t>
   </si>
   <si>
     <t>Production</t>
   </si>
   <si>
-    <t>Number of workers eviscerasion/portioning</t>
-  </si>
-  <si>
-    <t>Number of workers hanging</t>
-  </si>
-  <si>
-    <t>Number of workers clearing</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -226,13 +208,76 @@
   </si>
   <si>
     <t>proportion</t>
+  </si>
+  <si>
+    <t>Number of workers portioning</t>
+  </si>
+  <si>
+    <t>Number of workers clearing/thinning</t>
+  </si>
+  <si>
+    <t>Number of workers hanging broilers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of workers unloading broilers </t>
+  </si>
+  <si>
+    <t>n_unloading</t>
+  </si>
+  <si>
+    <t>Visite abattoire</t>
+  </si>
+  <si>
+    <t>n_post_bleeding</t>
+  </si>
+  <si>
+    <t>Number of workers inspecting post bleeding</t>
+  </si>
+  <si>
+    <t>n_post_ev</t>
+  </si>
+  <si>
+    <t>Number of workers inspecting post evisceration</t>
+  </si>
+  <si>
+    <t>n_post_df</t>
+  </si>
+  <si>
+    <t>Number of workers inspecting post defeathering</t>
+  </si>
+  <si>
+    <t>eff.post_bleeding</t>
+  </si>
+  <si>
+    <t>eff.post_df</t>
+  </si>
+  <si>
+    <t>machines</t>
+  </si>
+  <si>
+    <t>Inefficiency of bleeding machine</t>
+  </si>
+  <si>
+    <t>Inefficiency of defeathering machine</t>
+  </si>
+  <si>
+    <t>King et al. (2020)</t>
+  </si>
+  <si>
+    <t>n_portioning</t>
+  </si>
+  <si>
+    <t>crate_size</t>
+  </si>
+  <si>
+    <t>Number of broilers per crate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,19 +306,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +338,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -326,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -338,14 +378,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -676,7 +715,7 @@
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" customWidth="1"/>
     <col min="3" max="3" width="18.6328125" customWidth="1"/>
-    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="4" max="4" width="40.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7265625" customWidth="1"/>
     <col min="7" max="7" width="10.36328125" customWidth="1"/>
@@ -741,7 +780,7 @@
       <c r="A2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C2" t="s">
@@ -781,7 +820,7 @@
       <c r="A3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C3" t="s">
@@ -823,7 +862,7 @@
       <c r="A4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C4" t="s">
@@ -863,7 +902,7 @@
       <c r="A5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -905,17 +944,17 @@
       <c r="A6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>16</v>
@@ -938,21 +977,23 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6"/>
+      <c r="O6" t="s">
+        <v>75</v>
+      </c>
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
         <v>49</v>
@@ -976,200 +1017,335 @@
       <c r="O7" t="s">
         <v>50</v>
       </c>
-      <c r="P7" s="18" t="s">
-        <v>56</v>
+      <c r="P7" s="16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="3">
-        <v>3</v>
-      </c>
-      <c r="I8" s="3">
-        <v>13</v>
-      </c>
-      <c r="J8" s="3">
-        <v>6</v>
-      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="2"/>
+      <c r="L8">
+        <v>1</v>
+      </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="17" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
         <v>49</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="3">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I9" s="3">
-        <v>30</v>
-      </c>
-      <c r="J9" s="3"/>
-      <c r="L9"/>
+        <v>13</v>
+      </c>
+      <c r="J9" s="3">
+        <v>6</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
       <c r="O9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="P9" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="8"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="B10" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="2"/>
+      <c r="L10">
+        <v>1</v>
+      </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
+      <c r="O10" t="s">
+        <v>63</v>
+      </c>
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="8"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="A11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="2"/>
+      <c r="L11">
+        <v>1</v>
+      </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
+      <c r="O11" t="s">
+        <v>63</v>
+      </c>
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="A12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
+      <c r="I12" s="3">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="3"/>
+      <c r="O12" t="s">
+        <v>63</v>
+      </c>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+    <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="3">
+        <v>10</v>
+      </c>
+      <c r="I13" s="3">
+        <v>12</v>
+      </c>
       <c r="J13" s="3"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="2"/>
+      <c r="L13"/>
+      <c r="O13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P13" s="3"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="A14" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
+      <c r="L14">
+        <v>3.3000000000000002E-2</v>
+      </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="3"/>
+      <c r="O14" t="s">
+        <v>63</v>
+      </c>
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="A15" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+      <c r="L15">
+        <v>0.33</v>
+      </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="O15" s="3"/>
+      <c r="O15" t="s">
+        <v>63</v>
+      </c>
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="A16" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="L16" s="2">
+        <v>10</v>
+      </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
-      <c r="O16" s="3"/>
+      <c r="O16" t="s">
+        <v>63</v>
+      </c>
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
@@ -1178,16 +1354,17 @@
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
       <c r="J17" s="3"/>
+      <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
+      <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
@@ -1197,14 +1374,15 @@
       <c r="E18" s="9"/>
       <c r="F18" s="2"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="L18" s="3"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="3"/>
+      <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
@@ -1213,9 +1391,9 @@
       <c r="D19" s="10"/>
       <c r="E19" s="9"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1232,15 +1410,15 @@
       <c r="E20" s="9"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="3"/>
-      <c r="P20" s="5"/>
+      <c r="P20" s="2"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
@@ -1248,17 +1426,16 @@
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="2"/>
+      <c r="F21" s="3"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="3"/>
-      <c r="P21" s="5"/>
+      <c r="P21" s="3"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
@@ -1267,16 +1444,15 @@
       <c r="D22" s="10"/>
       <c r="E22" s="9"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="J22" s="3"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="2"/>
+      <c r="O22" s="3"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
@@ -1288,12 +1464,12 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="J23" s="3"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
-      <c r="O23" s="8"/>
+      <c r="O23" s="3"/>
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
@@ -1304,15 +1480,15 @@
       <c r="E24" s="9"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="2"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="5"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
@@ -1329,8 +1505,8 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="2"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="5"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
@@ -1340,9 +1516,9 @@
       <c r="E26" s="9"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
@@ -1350,23 +1526,41 @@
       <c r="O26" s="8"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="13"/>
-      <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="13"/>
-      <c r="G28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="O28" s="3"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
@@ -1375,62 +1569,52 @@
       <c r="D29" s="10"/>
       <c r="E29" s="9"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="3"/>
+      <c r="G29" s="2"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="2"/>
+      <c r="J29" s="3"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="3"/>
+      <c r="O29" s="8"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="13"/>
-      <c r="G30" s="3"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="11"/>
       <c r="O31" s="3"/>
-      <c r="P31" s="2"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="11"/>
+      <c r="G32" s="3"/>
+      <c r="J32" s="3"/>
       <c r="O32" s="3"/>
-      <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
@@ -1438,10 +1622,10 @@
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
       <c r="E33" s="9"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -1450,22 +1634,15 @@
       <c r="O33" s="3"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="11"/>
+      <c r="G34" s="3"/>
+      <c r="J34" s="3"/>
       <c r="O34" s="3"/>
-      <c r="P34" s="2"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
@@ -1485,13 +1662,23 @@
       <c r="O35" s="3"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="13"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
       <c r="O36" s="3"/>
+      <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
@@ -1499,10 +1686,11 @@
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="2"/>
+      <c r="F37" s="3"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
@@ -1517,7 +1705,7 @@
       <c r="D38" s="10"/>
       <c r="E38" s="9"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="3"/>
+      <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="K38" s="2"/>
@@ -1534,32 +1722,24 @@
       <c r="D39" s="10"/>
       <c r="E39" s="9"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="3"/>
+      <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-      <c r="L39" s="3"/>
+      <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="3"/>
       <c r="P39" s="2"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="11"/>
       <c r="O40" s="3"/>
-      <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
@@ -1568,10 +1748,9 @@
       <c r="D41" s="10"/>
       <c r="E41" s="9"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="3"/>
+      <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
@@ -1589,7 +1768,6 @@
       <c r="G42" s="3"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
@@ -1607,11 +1785,11 @@
       <c r="G43" s="3"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
+      <c r="L43" s="3"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
+      <c r="O43" s="3"/>
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
@@ -1624,11 +1802,11 @@
       <c r="G44" s="3"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
+      <c r="L44" s="3"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
+      <c r="O44" s="3"/>
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.35">
@@ -1646,6 +1824,7 @@
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
+      <c r="O45" s="3"/>
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.35">
@@ -1656,38 +1835,38 @@
       <c r="E46" s="9"/>
       <c r="F46" s="2"/>
       <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="L46" s="3"/>
+      <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
+      <c r="O46" s="3"/>
       <c r="P46" s="2"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="13"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="9"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="G47" s="3"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="L47" s="3"/>
+      <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
-      <c r="O47" s="3"/>
       <c r="P47" s="2"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="14"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="10"/>
       <c r="E48" s="9"/>
       <c r="F48" s="2"/>
       <c r="G48" s="3"/>
@@ -1695,20 +1874,27 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="L48" s="3"/>
+      <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
       <c r="P48" s="2"/>
     </row>
-    <row r="49" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="13"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="2"/>
       <c r="G49" s="3"/>
-      <c r="L49" s="3"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="P49" s="2"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
@@ -1718,11 +1904,11 @@
       <c r="E50" s="9"/>
       <c r="F50" s="2"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
+      <c r="L50" s="3"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="P50" s="2"/>
@@ -1730,53 +1916,47 @@
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="9"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="11"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
-      <c r="J51" s="3"/>
+      <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="3"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
+      <c r="O51" s="3"/>
       <c r="P51" s="2"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="10"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="12"/>
       <c r="E52" s="9"/>
       <c r="F52" s="2"/>
       <c r="G52" s="3"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
-      <c r="J52" s="3"/>
+      <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="3"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
       <c r="P52" s="2"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="2"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="11"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="P53" s="2"/>
+      <c r="L53" s="3"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
@@ -1807,7 +1987,7 @@
       <c r="I55" s="2"/>
       <c r="J55" s="3"/>
       <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
+      <c r="L55" s="3"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="P55" s="2"/>
@@ -1824,7 +2004,7 @@
       <c r="I56" s="2"/>
       <c r="J56" s="3"/>
       <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
+      <c r="L56" s="3"/>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="P56" s="2"/>
@@ -1839,7 +2019,7 @@
       <c r="G57" s="3"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
-      <c r="J57" s="3"/>
+      <c r="J57" s="2"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
@@ -1847,67 +2027,135 @@
       <c r="P57" s="2"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
+      <c r="P58" s="2"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="3"/>
       <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="P59" s="2"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="3"/>
       <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="P60" s="2"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="3"/>
       <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="P61" s="2"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="K62" s="2"/>
-      <c r="O62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="K63" s="2"/>
-      <c r="O63" s="2"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="O64" s="2"/>
+      <c r="K64" s="2"/>
+    </row>
+    <row r="65" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K65" s="2"/>
+    </row>
+    <row r="66" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K66" s="2"/>
+      <c r="O66" s="2"/>
+    </row>
+    <row r="67" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K67" s="2"/>
+      <c r="O67" s="2"/>
+    </row>
+    <row r="68" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="O68" s="2"/>
     </row>
   </sheetData>
   <dataValidations xWindow="721" yWindow="594" count="12">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K59:K63">
-      <formula1>I59</formula1>
-      <formula2>J59</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K63:K67">
+      <formula1>I63</formula1>
+      <formula2>J63</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O63">
-      <formula1>K63</formula1>
-      <formula2>L63</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O67">
+      <formula1>K67</formula1>
+      <formula2>L67</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K18:K57 K2:K16">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K22:K61 K2:K20">
       <formula1>I2</formula1>
       <formula2>J2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="P17">
-      <formula1>O17</formula1>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="P21">
+      <formula1>O21</formula1>
       <formula2>#REF!</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L35:L36 L41:L57 L2:L33"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="L38">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L39:L40 L45:L61 L2:L37"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="L42">
+      <formula1>H42</formula1>
+      <formula2>I42</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J39:J40 J45:J61 J2:J37">
+      <formula1>H2</formula1>
+      <formula2>I2</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="L43:L44 L41 L38">
       <formula1>H38</formula1>
       <formula2>I38</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J35:J36 J41:J57 J2:J33">
-      <formula1>H2</formula1>
-      <formula2>I2</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="L39:L40 L37 L34">
-      <formula1>H34</formula1>
-      <formula2>I34</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M57"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N57"/>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I57">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M61"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N61"/>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I61">
       <formula1>H2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H57">
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H61">
       <formula1>I2</formula1>
     </dataValidation>
   </dataValidations>
@@ -1920,13 +2168,13 @@
           <x14:formula1>
             <xm:f>ListItem!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G57</xm:sqref>
+          <xm:sqref>G2:G61</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution" prompt="Select a probability distribution">
           <x14:formula1>
             <xm:f>ListItem!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F57</xm:sqref>
+          <xm:sqref>F2:F61</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
fix: contact transmission per cm2
</commit_message>
<xml_diff>
--- a/data-input/estimated_variables.xlsx
+++ b/data-input/estimated_variables.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="82">
   <si>
     <t>Module</t>
   </si>
@@ -271,6 +271,15 @@
   </si>
   <si>
     <t>Number of broilers per crate</t>
+  </si>
+  <si>
+    <t>finger_surface</t>
+  </si>
+  <si>
+    <t>Surface area of worker's finger</t>
+  </si>
+  <si>
+    <t>cm2</t>
   </si>
 </sst>
 </file>
@@ -704,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P68"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1240,41 +1249,39 @@
       </c>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
+      <c r="B14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" t="s">
-        <v>63</v>
-      </c>
-      <c r="P14" s="2"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3">
+        <v>1.71</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="L14"/>
+      <c r="O14"/>
+      <c r="P14" s="3"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
@@ -1283,11 +1290,11 @@
       <c r="B15" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>71</v>
+      <c r="C15" t="s">
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
         <v>57</v>
@@ -1303,7 +1310,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15">
-        <v>0.33</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1319,14 +1326,14 @@
       <c r="B16" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>78</v>
+      <c r="C16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>11</v>
@@ -1338,8 +1345,8 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="2">
-        <v>10</v>
+      <c r="L16">
+        <v>0.33</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1349,21 +1356,39 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="A17" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="L17" s="2">
+        <v>10</v>
+      </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
-      <c r="O17" s="3"/>
+      <c r="O17" t="s">
+        <v>63</v>
+      </c>
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
@@ -1378,7 +1403,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="3"/>
+      <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="3"/>
@@ -1396,7 +1421,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
+      <c r="L19" s="3"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="3"/>
@@ -1409,10 +1434,10 @@
       <c r="D20" s="10"/>
       <c r="E20" s="9"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -1426,16 +1451,17 @@
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="3"/>
+      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
+      <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
@@ -1443,16 +1469,16 @@
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
@@ -1461,7 +1487,7 @@
       <c r="D23" s="10"/>
       <c r="E23" s="9"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="3"/>
@@ -1470,7 +1496,6 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
@@ -1480,15 +1505,15 @@
       <c r="E24" s="9"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
       <c r="J24" s="3"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="5"/>
+      <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
@@ -1516,15 +1541,15 @@
       <c r="E26" s="9"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="2"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="5"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
@@ -1570,9 +1595,9 @@
       <c r="E29" s="9"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -1598,13 +1623,23 @@
       <c r="O30" s="8"/>
       <c r="P30" s="2"/>
     </row>
-    <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="11"/>
-      <c r="O31" s="3"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
@@ -1612,55 +1647,45 @@
       <c r="C32" s="11"/>
       <c r="D32" s="12"/>
       <c r="E32" s="11"/>
-      <c r="G32" s="3"/>
-      <c r="J32" s="3"/>
       <c r="O32" s="3"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="2"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="11"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="J33" s="3"/>
       <c r="O33" s="3"/>
-      <c r="P33" s="2"/>
-    </row>
-    <row r="34" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="11"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="2"/>
       <c r="G34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
       <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="11"/>
+      <c r="G35" s="3"/>
+      <c r="J35" s="3"/>
       <c r="O35" s="3"/>
-      <c r="P35" s="2"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
@@ -1686,7 +1711,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="3"/>
+      <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -1704,10 +1729,11 @@
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="2"/>
+      <c r="F38" s="3"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
@@ -1725,7 +1751,6 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
@@ -1733,30 +1758,31 @@
       <c r="O39" s="3"/>
       <c r="P39" s="2"/>
     </row>
-    <row r="40" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="11"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
       <c r="O40" s="3"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P40" s="2"/>
+    </row>
+    <row r="41" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="11"/>
       <c r="O41" s="3"/>
-      <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
@@ -1765,7 +1791,7 @@
       <c r="D42" s="10"/>
       <c r="E42" s="9"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="3"/>
+      <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="K42" s="2"/>
@@ -1786,7 +1812,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="3"/>
+      <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="3"/>
@@ -1819,9 +1845,8 @@
       <c r="G45" s="3"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
+      <c r="L45" s="3"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="3"/>
@@ -1860,6 +1885,7 @@
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
+      <c r="O47" s="3"/>
       <c r="P47" s="2"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
@@ -1904,11 +1930,11 @@
       <c r="E50" s="9"/>
       <c r="F50" s="2"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="L50" s="3"/>
+      <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="P50" s="2"/>
@@ -1916,19 +1942,18 @@
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="11"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="9"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="3"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
-      <c r="O51" s="3"/>
       <c r="P51" s="2"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
@@ -1936,9 +1961,9 @@
       <c r="B52" s="3"/>
       <c r="C52" s="11"/>
       <c r="D52" s="12"/>
-      <c r="E52" s="9"/>
+      <c r="E52" s="11"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="3"/>
+      <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -1946,34 +1971,35 @@
       <c r="L52" s="3"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
+      <c r="O52" s="3"/>
       <c r="P52" s="2"/>
     </row>
-    <row r="53" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="11"/>
       <c r="D53" s="12"/>
-      <c r="E53" s="11"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="2"/>
       <c r="G53" s="3"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
       <c r="L53" s="3"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+    </row>
+    <row r="54" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="2"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="11"/>
       <c r="G54" s="3"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="P54" s="2"/>
+      <c r="L54" s="3"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
@@ -1987,7 +2013,7 @@
       <c r="I55" s="2"/>
       <c r="J55" s="3"/>
       <c r="K55" s="2"/>
-      <c r="L55" s="3"/>
+      <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="P55" s="2"/>
@@ -2019,9 +2045,9 @@
       <c r="G57" s="3"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
+      <c r="J57" s="3"/>
       <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
+      <c r="L57" s="3"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
       <c r="P57" s="2"/>
@@ -2036,7 +2062,7 @@
       <c r="G58" s="3"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
-      <c r="J58" s="3"/>
+      <c r="J58" s="2"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
@@ -2095,12 +2121,26 @@
       <c r="P61" s="2"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="2"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
+      <c r="P62" s="2"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="K64" s="2"/>
@@ -2110,52 +2150,55 @@
     </row>
     <row r="66" spans="11:15" x14ac:dyDescent="0.35">
       <c r="K66" s="2"/>
-      <c r="O66" s="2"/>
     </row>
     <row r="67" spans="11:15" x14ac:dyDescent="0.35">
       <c r="K67" s="2"/>
       <c r="O67" s="2"/>
     </row>
     <row r="68" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K68" s="2"/>
       <c r="O68" s="2"/>
+    </row>
+    <row r="69" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="O69" s="2"/>
     </row>
   </sheetData>
   <dataValidations xWindow="721" yWindow="594" count="12">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K63:K67">
-      <formula1>I63</formula1>
-      <formula2>J63</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot;" sqref="K64:K68">
+      <formula1>I64</formula1>
+      <formula2>J64</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O67">
-      <formula1>K67</formula1>
-      <formula2>L67</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. This cell must remain empty when the selected probability distribution is &quot;Uniform&quot;_x000a_" sqref="O68">
+      <formula1>K68</formula1>
+      <formula2>L68</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K22:K61 K2:K20">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="K23:K62 K2:K21">
       <formula1>I2</formula1>
       <formula2>J2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="P21">
-      <formula1>O21</formula1>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="P22">
+      <formula1>O22</formula1>
       <formula2>#REF!</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L39:L40 L45:L61 L2:L37"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="L42">
-      <formula1>H42</formula1>
-      <formula2>I42</formula2>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution, which had not been covered by the previous columns. Examples: value of the &quot;Point estimate&quot; variable, parameters of &quot;Poisson&quot; or &quot;NegBin&quot; (negative binomial) distributions" sqref="L40:L41 L46:L62 L2:L38"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Standard deviation" prompt="Enter the standard deviation of the mean of the probability distribution. This cell must be filled only when the selected probability distribution is &quot;Normal&quot; or &quot;LogNormal&quot;" sqref="L43">
+      <formula1>H43</formula1>
+      <formula2>I43</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J39:J40 J45:J61 J2:J37">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="J40:J41 J46:J62 J2:J38">
       <formula1>H2</formula1>
       <formula2>I2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="L43:L44 L41 L38">
-      <formula1>H38</formula1>
-      <formula2>I38</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMean" error="Something is wrong. Please enter a value between the minimum and maximum values" promptTitle="Mean" prompt="Enter the most likely value (or mean value) of the probability distribution. _x000a_" sqref="L44:L45 L42 L39">
+      <formula1>H39</formula1>
+      <formula2>I39</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M61"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N61"/>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I61">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: second shape parameter of the Beta distribution_x000a_" sqref="M2:M62"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Other3" prompt="Enter the parameter of the probability distribution not covered by the previous columns. Examples: shift parameter of the shifted log logistic distribution_x000a_" sqref="N2:N62"/>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMax" error="Something is wrong. Are you sure the value you entered is the maximal value?" promptTitle="Maximum" prompt="Enter the maximal value of the probability distribution. This cell can be also used to define the upper bound of truncated distributions." sqref="I2:I62">
       <formula1>H2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H61">
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ErrorMin" error="Something is wrong. Are you sure the value you entered is the minimum value?" promptTitle="Minimum" prompt="Enter Minimal value of the probability distribution. This cell can be also used to defined the lower bound of truncated distributions." sqref="H2:H62">
       <formula1>I2</formula1>
     </dataValidation>
   </dataValidations>
@@ -2168,13 +2211,13 @@
           <x14:formula1>
             <xm:f>ListItem!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G61</xm:sqref>
+          <xm:sqref>G2:G62</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distribution" prompt="Select a probability distribution">
           <x14:formula1>
             <xm:f>ListItem!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F61</xm:sqref>
+          <xm:sqref>F2:F62</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>